<commit_message>
Updated all endpoint tests
</commit_message>
<xml_diff>
--- a/util/development-requests/Tspec-DVU-Casus.xlsx
+++ b/util/development-requests/Tspec-DVU-Casus.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HHS-Group-3-DVU\util\development-requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DDBAE5-6EB7-4B9C-B90D-1175DB6726D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6BC7E0-0AFF-402F-B99B-CC259646EA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="15600" activeTab="2" xr2:uid="{F887C0C3-FFB6-426A-9BD0-08BBB2E77D56}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F887C0C3-FFB6-426A-9BD0-08BBB2E77D56}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
     <sheet name="Gebruikers" sheetId="2" r:id="rId2"/>
-    <sheet name="endpionts-backend" sheetId="5" r:id="rId3"/>
+    <sheet name="endpoints-backend" sheetId="5" r:id="rId3"/>
     <sheet name="Tspec01" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Beschrijving</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>De test casus heeft als focus om alle endpionts te testen die geen data genereren op de sessie token na.</t>
-  </si>
-  <si>
-    <t>Kolom2</t>
   </si>
   <si>
     <t>Id</t>
@@ -254,13 +251,19 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>#68</t>
+  </si>
+  <si>
+    <t>Bugs - azure link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +287,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +345,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -513,10 +530,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -526,102 +544,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -636,11 +558,109 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -655,9 +675,7 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -666,6 +684,251 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE8F2A1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -699,249 +962,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE8F2A1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -961,19 +981,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0523BD7-A6CF-44DE-8E4E-08A126ACCA76}" name="Tabel1" displayName="Tabel1" ref="A12:J29" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0523BD7-A6CF-44DE-8E4E-08A126ACCA76}" name="Tabel1" displayName="Tabel1" ref="A12:J29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="A12:J29" xr:uid="{E0523BD7-A6CF-44DE-8E4E-08A126ACCA76}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{007A3CB7-2103-4D91-87BE-BBDA6DDA2D75}" name="Id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B2342056-0644-4895-A9B7-A79D483AEF3C}" name="Wizard" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{40A3833E-B7D9-449D-9569-EABCF1073CEE}" name="Test-object" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E4201C9C-2269-4528-BC18-E9479B9CFDFD}" name="HTTP type" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{B53DD4EE-F856-4AAC-B5DC-F2FCD678781D}" name="File name(s)*" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{9D3D4E5A-81A8-41FC-97AD-9EEABA718E51}" name="Query Params" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{47F73B45-6F58-43AB-9AE3-EAA4BB5B8BCD}" name="UserTypes" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{2F367C1B-94B3-4FB9-84D8-293029B1C6D8}" name="URL extension" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{D5177B5B-5D31-4F15-8A4C-BC57C63DFC09}" name="Requires Authentication" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{F31974CB-5691-42F7-A49C-198929E8A488}" name="Kolom2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{007A3CB7-2103-4D91-87BE-BBDA6DDA2D75}" name="Id" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B2342056-0644-4895-A9B7-A79D483AEF3C}" name="Wizard" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{40A3833E-B7D9-449D-9569-EABCF1073CEE}" name="Test-object" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E4201C9C-2269-4528-BC18-E9479B9CFDFD}" name="HTTP type" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{B53DD4EE-F856-4AAC-B5DC-F2FCD678781D}" name="File name(s)*" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{9D3D4E5A-81A8-41FC-97AD-9EEABA718E51}" name="Query Params" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{47F73B45-6F58-43AB-9AE3-EAA4BB5B8BCD}" name="UserTypes" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{2F367C1B-94B3-4FB9-84D8-293029B1C6D8}" name="URL extension" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D5177B5B-5D31-4F15-8A4C-BC57C63DFC09}" name="Requires Authentication" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{F31974CB-5691-42F7-A49C-198929E8A488}" name="Bugs - azure link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1370,17 +1390,17 @@
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -1565,7 +1585,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1599,7 @@
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="29.28515625" customWidth="1"/>
     <col min="9" max="9" width="24.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1593,74 +1613,74 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="B8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -1687,47 +1707,47 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="49" t="s">
+      <c r="A12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="49" t="s">
+      <c r="F12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="50" t="s">
-        <v>40</v>
+      <c r="J12" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>46</v>
+      <c r="B13" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="3" t="s">
@@ -1737,10 +1757,10 @@
         <v>29</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="J13" s="43"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
@@ -1756,7 +1776,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>27</v>
@@ -1770,65 +1790,67 @@
       <c r="I14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="44"/>
+      <c r="J14" s="52" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>3</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>47</v>
+      <c r="B15" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="43"/>
+        <v>48</v>
+      </c>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="44"/>
+        <v>48</v>
+      </c>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>5</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>47</v>
+      <c r="B17" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>28</v>
@@ -1837,116 +1859,116 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="43"/>
+        <v>48</v>
+      </c>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="44"/>
+        <v>48</v>
+      </c>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>7</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="43"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="44"/>
+        <v>48</v>
+      </c>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>9</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="43"/>
+        <v>48</v>
+      </c>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>10</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>28</v>
@@ -1955,58 +1977,58 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="44"/>
+        <v>48</v>
+      </c>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>11</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="43"/>
+        <v>48</v>
+      </c>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="44"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -2020,7 +2042,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="43"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -2034,7 +2056,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="44"/>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -2048,7 +2070,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="43"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -2062,21 +2084,21 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="44"/>
+      <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="45">
+      <c r="A29" s="13">
         <v>17</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2085,9 +2107,12 @@
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J14" r:id="rId1" xr:uid="{1AB078C8-3712-4B84-9B2D-A08DDA15F124}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2096,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5069E249-2935-4640-ABCE-686A53E64DC7}">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,48 +2140,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2179,12 +2204,12 @@
       <c r="G6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="21"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -2334,115 +2359,115 @@
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="28"/>
+      <c r="B17" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="29"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="29"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="29"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>15</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="29"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>16</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="29"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>17</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="29"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="41"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>18</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="29"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="41"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>19</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="29"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="41"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>20</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="30"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -2558,101 +2583,101 @@
       <c r="A37" s="5">
         <v>31</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="28"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>32</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="29"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="41"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>33</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="29"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="41"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>34</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="29"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="41"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>35</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="29"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="41"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="29"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="41"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="29"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="41"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="29"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="41"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="29"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="41"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="30"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="42"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -2740,6 +2765,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G37:G46"/>
+    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="C27:C36"/>
+    <mergeCell ref="D27:D36"/>
+    <mergeCell ref="E27:E36"/>
+    <mergeCell ref="F27:F36"/>
+    <mergeCell ref="G27:G36"/>
+    <mergeCell ref="B37:B46"/>
+    <mergeCell ref="C37:C46"/>
+    <mergeCell ref="D37:D46"/>
+    <mergeCell ref="E37:E46"/>
+    <mergeCell ref="F37:F46"/>
+    <mergeCell ref="G17:G26"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="B17:B26"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="D17:D26"/>
+    <mergeCell ref="E17:E26"/>
+    <mergeCell ref="F17:F26"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="B7:B16"/>
@@ -2748,28 +2795,6 @@
     <mergeCell ref="E7:E16"/>
     <mergeCell ref="F7:F16"/>
     <mergeCell ref="G7:G16"/>
-    <mergeCell ref="B17:B26"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="D17:D26"/>
-    <mergeCell ref="E17:E26"/>
-    <mergeCell ref="F17:F26"/>
-    <mergeCell ref="G17:G26"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="B37:B46"/>
-    <mergeCell ref="C37:C46"/>
-    <mergeCell ref="D37:D46"/>
-    <mergeCell ref="E37:E46"/>
-    <mergeCell ref="F37:F46"/>
-    <mergeCell ref="G37:G46"/>
-    <mergeCell ref="B27:B36"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="D27:D36"/>
-    <mergeCell ref="E27:E36"/>
-    <mergeCell ref="F27:F36"/>
-    <mergeCell ref="G27:G36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>